<commit_message>
OC 12 lavet, og tidsregistrering er opdaterert
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet(Tolga).xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet(Tolga).xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="81">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -632,7 +632,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -640,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,8 +1163,14 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>42814</v>
+      </c>
+      <c r="B31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sidste opdatering af tidsregistrering
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet(Tolga).xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet(Tolga).xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="93">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -296,6 +296,15 @@
   </si>
   <si>
     <t>GUI, videre arbejde og rettelser på mellemregninger</t>
+  </si>
+  <si>
+    <t>Test for flydespaending</t>
+  </si>
+  <si>
+    <t>Test Analysist</t>
+  </si>
+  <si>
+    <t>Test for dimensionerende kraft(Ikke færdig)</t>
   </si>
 </sst>
 </file>
@@ -667,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="D34" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,7 +1085,7 @@
         <v>55</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="F25" t="s">
         <v>73</v>
@@ -1096,7 +1105,7 @@
         <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="F26" t="s">
         <v>74</v>
@@ -1202,7 +1211,7 @@
         <v>55</v>
       </c>
       <c r="D33" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="F33" t="s">
         <v>81</v>
@@ -1325,7 +1334,7 @@
         <v>55</v>
       </c>
       <c r="D40" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="F40" t="s">
         <v>87</v>
@@ -1345,7 +1354,7 @@
         <v>55</v>
       </c>
       <c r="D41" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="F41" t="s">
         <v>88</v>
@@ -1365,7 +1374,7 @@
         <v>55</v>
       </c>
       <c r="D42" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="F42" t="s">
         <v>89</v>
@@ -1378,6 +1387,49 @@
       </c>
       <c r="I42">
         <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B44" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
+        <v>90</v>
+      </c>
+      <c r="G44" s="5">
+        <v>0.34375</v>
+      </c>
+      <c r="H44" s="5">
+        <v>0.3923611111111111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B45" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" t="s">
+        <v>92</v>
+      </c>
+      <c r="G45" s="5">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="H45" s="5">
+        <v>0.43402777777777773</v>
+      </c>
+      <c r="I45">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test for DimensionerendeKraft oprettet, og opdatering af
tidsregistrering
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet(Tolga).xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet(Tolga).xlsx
@@ -304,7 +304,7 @@
     <t>Test Analysist</t>
   </si>
   <si>
-    <t>Test for dimensionerende kraft(Ikke færdig)</t>
+    <t>Test for dimensionerende kraft</t>
   </si>
 </sst>
 </file>
@@ -668,7 +668,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -678,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D34" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="D40" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>